<commit_message>
changed chat to list
</commit_message>
<xml_diff>
--- a/Modules/backend/API_table.xlsx
+++ b/Modules/backend/API_table.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B71194D-9C02-4212-9663-D9CCCD9A48E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2754D1-5F4C-4905-A487-3832C0FAE015}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API Documentation" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="178">
   <si>
     <t>Server URL</t>
   </si>
@@ -1626,24 +1626,6 @@
 }</t>
   </si>
   <si>
-    <t>var unirest = require("unirest");
-var req = unirest("POST", "https://courier50003.herokuapp.com/portal/usersubmitacc");
-req.headers({
-  "cache-control": "no-cache",
-  "content-type": "application/json"
-});
-req.type("json");
-req.send({
-  "id": "5c9b628a46d6b239c07fcffd",
-  "message": "I have a problem with my API service request that I could not solve. When can you get back to me with save me an answer. This is not so urgent",
-  "category": "test"
-});
-req.end(function (res) {
-  if (res.error) throw new Error(res.error);
-  console.log(res.body);
-});</t>
-  </si>
-  <si>
     <t>{
     "success": true,
     "name": "tututtu",
@@ -1662,6 +1644,112 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> [
+        {
+            "date": "2019-03-22T04:31:11.057Z",
+            "_id": "5c94650f471b590004e5fd06",
+            "name": "caleb",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T04:31:38.184Z",
+            "_id": "5c94652a471b590004e5fd07",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T04:38:26.839Z",
+            "_id": "5c9466c2471b590004e5fd08",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T04:39:06.492Z",
+            "_id": "5c9466ea471b590004e5fd09",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T04:39:22.935Z",
+            "_id": "5c9466fa471b590004e5fd0a",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T04:40:52.977Z",
+            "_id": "5c946754471b590004e5fd0b",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T04:41:40.643Z",
+            "_id": "5c946784471b590004e5fd0c",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T04:43:20.398Z",
+            "_id": "5c9467e8471b590004e5fd0d",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T04:44:49.263Z",
+            "_id": "5c946841471b590004e5fd0e",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T04:46:51.803Z",
+            "_id": "5c9468bb471b590004e5fd0f",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T04:48:06.196Z",
+            "_id": "5c946906471b590004e5fd10",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T08:03:35.102Z",
+            "_id": "5c9496d7d290ed0004afefa4",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T08:03:38.945Z",
+            "_id": "5c9496dad290ed0004afefa5",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T08:03:49.210Z",
+            "_id": "5c9496e5d290ed0004afefa6",
+            "name": "admin1",
+            "message": "Hello world i am testing again"
+        },
+        {
+            "date": "2019-03-22T08:26:07.766Z",
+            "_id": "5c949c1f0c04570004482ecd",
+            "name": "admin1",
+            "message": "bye bye"
+        },
+        {
+            "date": "2019-03-22T08:27:14.205Z",
+            "_id": "5c949c620c04570004482ece",
+            "name": "admin1",
+            "message": "holy shit"
+        },
+        {
+            "date": "2019-03-22T08:59:14.169Z",
+            "_id": "5c94a3e20c04570004482ed9",
+            "name": "admin1",
+            "message": "how can i help you?"
+        }
+    ]</t>
+  </si>
+  <si>
     <t>var unirest = require("unirest");
 var req = unirest("POST", "https://courier50003.herokuapp.com/portal/usersubmit");
 req.headers({
@@ -1671,6 +1759,7 @@
 req.type("json");
 req.send({
   "name": "tututtu",
+  "title":"sample",
   "message": "I have a problem with my API service request that I could not solve. When can you get back to me with save me an answer. This is not so urgent",
   "contact_num": 92929323,
   "category": "fun",
@@ -1680,6 +1769,48 @@
   if (res.error) throw new Error(res.error);
   console.log(res.body);
 });</t>
+  </si>
+  <si>
+    <t>var unirest = require("unirest");
+var req = unirest("POST", "https://courier50003.herokuapp.com/portal/usersubmitacc");
+req.headers({
+  "cache-control": "no-cache",
+  "content-type": "application/json"
+});
+req.type("json");
+req.send({
+  "id": "5c9b628a46d6b239c07fcffd",
+  "title":"sample",
+  "message": "I have a problem with my API service request that I could not solve. When can you get back to me with save me an answer. This is not so urgent",
+  "category": "test"
+});
+req.end(function (res) {
+  if (res.error) throw new Error(res.error);
+  console.log(res.body);
+});</t>
+  </si>
+  <si>
+    <t>1) username: String
+2) message: String
+3) contact_num: Long
+4) img: PNG/JPG
+5) category: String
+6) email: String
+6) sentiment: Int
+7) tags: Array of Strings 
+8) name: String
+9) title: String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) name: String
+2) message: String
+3) contact_num: Long
+4) img: PNG/JPG
+5) category: String
+6) email: String
+6) sentiment: Int
+7) tags: Array of Strings
+8) title: String </t>
   </si>
 </sst>
 </file>
@@ -1833,6 +1964,27 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1843,27 +1995,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2145,10 +2276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62BDFB2-F4C2-4F33-9912-B3BD4F1C0B04}">
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="41" zoomScaleNormal="41" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2295,7 +2426,7 @@
       <c r="N6" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="11" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2444,7 +2575,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:16" ht="403.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -2455,10 +2586,10 @@
         <v>174</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>177</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>113</v>
@@ -2481,7 +2612,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="374.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -2489,10 +2620,10 @@
         <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>176</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>171</v>
@@ -2500,10 +2631,10 @@
       <c r="F14" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="10" t="s">
         <v>134</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -2537,10 +2668,10 @@
       <c r="F15" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="10" t="s">
         <v>124</v>
       </c>
       <c r="I15" s="2" t="s">
@@ -2572,10 +2703,10 @@
       <c r="F16" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="10" t="s">
         <v>124</v>
       </c>
       <c r="I16" s="2" t="s">
@@ -2607,10 +2738,10 @@
       <c r="F17" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="10" t="s">
         <v>135</v>
       </c>
       <c r="I17" s="2" t="s">
@@ -2630,14 +2761,14 @@
       <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="18"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="18"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="10"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -2665,10 +2796,10 @@
       <c r="F19" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="10" t="s">
         <v>149</v>
       </c>
       <c r="I19" s="2" t="s">
@@ -2698,16 +2829,16 @@
       <c r="D20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="14" t="s">
         <v>156</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H20" s="14"/>
+      <c r="H20" s="10"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -2729,14 +2860,14 @@
       <c r="D21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="17"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H21" s="14"/>
+      <c r="H21" s="10"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -2758,14 +2889,14 @@
       <c r="D22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="17"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H22" s="14"/>
+      <c r="H22" s="10"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -2787,14 +2918,14 @@
       <c r="D23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="17"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H23" s="14"/>
+      <c r="H23" s="10"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -2803,7 +2934,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="342.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -2816,14 +2947,14 @@
       <c r="D24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="13" t="s">
         <v>163</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G24" s="13"/>
-      <c r="H24" s="14"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="10"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -2831,6 +2962,11 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="E25" s="11" t="s">
+        <v>173</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3020,10 +3156,10 @@
       <c r="D13" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="17" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3040,8 +3176,8 @@
       <c r="D14" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="11"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -3056,8 +3192,8 @@
       <c r="D15" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="11"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -3072,8 +3208,8 @@
       <c r="D16" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="11"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -3088,8 +3224,8 @@
       <c r="D17" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="11"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -3104,8 +3240,8 @@
       <c r="D18" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="11"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -3120,8 +3256,8 @@
       <c r="D19" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="11"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -3136,8 +3272,8 @@
       <c r="D20" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="11"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -3152,8 +3288,8 @@
       <c r="D21" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="11"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -3168,8 +3304,8 @@
       <c r="D22" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="11"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -3184,8 +3320,8 @@
       <c r="D23" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="11"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -3200,8 +3336,8 @@
       <c r="D24" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="9"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>